<commit_message>
Traversing rows and columns of excel worksheet with excelJS library
</commit_message>
<xml_diff>
--- a/tests/excelDemo/exceldownload.xlsx
+++ b/tests/excelDemo/exceldownload.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\playwright-udemy\tests\excelDemo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A699D76-8DBF-41B6-8800-D379465E1ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D60DBD-3395-41C5-860F-8C0F161F9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -529,4 +530,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0883C51-457B-4224-966B-CBFE70AF72D2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Build Util function to read and update excel file strategically
</commit_message>
<xml_diff>
--- a/tests/excelDemo/exceldownload.xlsx
+++ b/tests/excelDemo/exceldownload.xlsx
@@ -1,14 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\playwright-udemy\tests\excelDemo\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D60DBD-3395-41C5-860F-8C0F161F9902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27932"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B44507D-C72B-41AD-B66B-D6520393B68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +11,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
       <xlwcv:version setVersion="1"/>
     </ext>
@@ -46,43 +38,43 @@
     <t>season</t>
   </si>
   <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
     <t>Summer</t>
   </si>
   <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
     <t>Winter</t>
   </si>
   <si>
+    <t>Papaya</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
     <t>Spring</t>
   </si>
   <si>
+    <t>Republic</t>
+  </si>
+  <si>
     <t>All</t>
   </si>
   <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>Orange</t>
+    <t>Kivi</t>
   </si>
   <si>
     <t>Green</t>
-  </si>
-  <si>
-    <t>Mango</t>
-  </si>
-  <si>
-    <t>Apple</t>
-  </si>
-  <si>
-    <t>Papaya</t>
-  </si>
-  <si>
-    <t>Banana</t>
-  </si>
-  <si>
-    <t>Kivi</t>
   </si>
 </sst>
 </file>
@@ -402,8 +394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,16 +422,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D2">
         <v>299</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -447,16 +439,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>345</v>
       </c>
       <c r="E3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -464,16 +456,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
         <v>187</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -481,16 +473,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D5">
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -498,16 +490,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
       <c r="D6">
         <v>399</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -515,16 +507,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7">
         <v>199</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -533,10 +525,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0883C51-457B-4224-966B-CBFE70AF72D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>